<commit_message>
Revise variables.metadata.autogenerate.R to add two metadata items, number of filter variables for each variable (nfv) and whether the universe involves a logical disjunction ('or').
And some metadata files for bolivia2001, which spurred the change because the economic activity questions involve a logical disjunction, breaking the simple model of universe = conjunction of filter variables with values in range.
</commit_message>
<xml_diff>
--- a/samples/bolivia2001/metadata/variables.metadata.manuallyedited.xlsx
+++ b/samples/bolivia2001/metadata/variables.metadata.manuallyedited.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="290">
   <si>
     <t>vdescription</t>
   </si>
@@ -782,6 +782,108 @@
   </si>
   <si>
     <t>P34</t>
+  </si>
+  <si>
+    <t>P35</t>
+  </si>
+  <si>
+    <t>P36</t>
+  </si>
+  <si>
+    <t>P37</t>
+  </si>
+  <si>
+    <t>P38</t>
+  </si>
+  <si>
+    <t>4:98</t>
+  </si>
+  <si>
+    <t>2:3</t>
+  </si>
+  <si>
+    <t>P39.1</t>
+  </si>
+  <si>
+    <t>P39.2</t>
+  </si>
+  <si>
+    <t>P39.1-2</t>
+  </si>
+  <si>
+    <t>P41</t>
+  </si>
+  <si>
+    <t>P40.1</t>
+  </si>
+  <si>
+    <t>P40.2</t>
+  </si>
+  <si>
+    <t>11:17</t>
+  </si>
+  <si>
+    <t>P42</t>
+  </si>
+  <si>
+    <t>7:98</t>
+  </si>
+  <si>
+    <t>P43</t>
+  </si>
+  <si>
+    <t>P44</t>
+  </si>
+  <si>
+    <t>P45</t>
+  </si>
+  <si>
+    <t>P46</t>
+  </si>
+  <si>
+    <t>P47</t>
+  </si>
+  <si>
+    <t>P48</t>
+  </si>
+  <si>
+    <t>P49</t>
+  </si>
+  <si>
+    <t>P50</t>
+  </si>
+  <si>
+    <t>P51</t>
+  </si>
+  <si>
+    <t>P52</t>
+  </si>
+  <si>
+    <t>P53.1</t>
+  </si>
+  <si>
+    <t>P53.2</t>
+  </si>
+  <si>
+    <t>P54</t>
+  </si>
+  <si>
+    <t>P55</t>
+  </si>
+  <si>
+    <t>15:98</t>
+  </si>
+  <si>
+    <t>P42=1 | (P42=2 &amp; P43=1:4)</t>
+  </si>
+  <si>
+    <t>nfv</t>
+  </si>
+  <si>
+    <t>disj</t>
+  </si>
+  <si>
+    <t>expression</t>
   </si>
 </sst>
 </file>
@@ -845,7 +947,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
@@ -860,6 +962,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1159,37 +1273,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S90"/>
+  <dimension ref="A1:V90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1222,33 +1340,42 @@
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="2" t="s">
+      <c r="V1" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1263,8 +1390,8 @@
       <c r="E2" s="3">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>196</v>
+      <c r="F2" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G2" s="3">
         <v>210471</v>
@@ -1281,12 +1408,8 @@
       <c r="K2" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
         <v>196</v>
       </c>
@@ -1305,9 +1428,15 @@
       <c r="S2" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="2" t="s">
+      <c r="T2" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1322,8 +1451,8 @@
       <c r="E3" s="3">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>196</v>
+      <c r="F3" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G3" s="3">
         <v>210471</v>
@@ -1340,12 +1469,8 @@
       <c r="K3" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
         <v>196</v>
       </c>
@@ -1364,9 +1489,15 @@
       <c r="S3" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="2" t="s">
+      <c r="T3" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1381,8 +1512,8 @@
       <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>196</v>
+      <c r="F4" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G4" s="3">
         <v>30</v>
@@ -1399,12 +1530,8 @@
       <c r="K4" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
       <c r="N4" s="5" t="s">
         <v>196</v>
       </c>
@@ -1423,9 +1550,15 @@
       <c r="S4" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="2" t="s">
+      <c r="T4" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1440,8 +1573,8 @@
       <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>196</v>
+      <c r="F5" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
@@ -1458,12 +1591,8 @@
       <c r="K5" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="5" t="s">
         <v>196</v>
       </c>
@@ -1482,9 +1611,15 @@
       <c r="S5" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="2" t="s">
+      <c r="T5" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1499,8 +1634,8 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>196</v>
+      <c r="F6" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G6" s="3">
         <v>9</v>
@@ -1517,12 +1652,8 @@
       <c r="K6" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="5" t="s">
         <v>196</v>
       </c>
@@ -1541,9 +1672,15 @@
       <c r="S6" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="2" t="s">
+      <c r="T6" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1558,8 +1695,8 @@
       <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>196</v>
+      <c r="F7" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G7" s="3">
         <v>14</v>
@@ -1576,12 +1713,8 @@
       <c r="K7" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
       <c r="N7" s="5" t="s">
         <v>196</v>
       </c>
@@ -1600,9 +1733,15 @@
       <c r="S7" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="2" t="s">
+      <c r="T7" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1617,8 +1756,8 @@
       <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>196</v>
+      <c r="F8" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G8" s="3">
         <v>2</v>
@@ -1635,12 +1774,8 @@
       <c r="K8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="5" t="s">
         <v>196</v>
       </c>
@@ -1659,9 +1794,15 @@
       <c r="S8" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="2" t="s">
+      <c r="T8" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1676,8 +1817,8 @@
       <c r="E9" s="3">
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>196</v>
+      <c r="F9" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
@@ -1694,12 +1835,8 @@
       <c r="K9" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="5" t="s">
         <v>196</v>
       </c>
@@ -1718,9 +1855,15 @@
       <c r="S9" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="2" t="s">
+      <c r="T9" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1735,8 +1878,8 @@
       <c r="E10" s="3">
         <v>1</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>196</v>
+      <c r="F10" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G10" s="3">
         <v>3</v>
@@ -1753,12 +1896,8 @@
       <c r="K10" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="5" t="s">
         <v>196</v>
       </c>
@@ -1777,9 +1916,15 @@
       <c r="S10" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="2" t="s">
+      <c r="T10" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1794,8 +1939,8 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>196</v>
+      <c r="F11" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G11" s="3">
         <v>6</v>
@@ -1812,12 +1957,8 @@
       <c r="K11" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
       <c r="N11" s="5" t="s">
         <v>196</v>
       </c>
@@ -1836,9 +1977,15 @@
       <c r="S11" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="2" t="s">
+      <c r="T11" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1853,8 +2000,8 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>196</v>
+      <c r="F12" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G12" s="3">
         <v>9</v>
@@ -1871,12 +2018,8 @@
       <c r="K12" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
       <c r="N12" s="5" t="s">
         <v>196</v>
       </c>
@@ -1895,9 +2038,15 @@
       <c r="S12" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="2" t="s">
+      <c r="T12" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1912,8 +2061,8 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>196</v>
+      <c r="F13" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G13" s="3">
         <v>9</v>
@@ -1930,12 +2079,8 @@
       <c r="K13" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
       <c r="N13" s="5" t="s">
         <v>196</v>
       </c>
@@ -1954,9 +2099,15 @@
       <c r="S13" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="2" t="s">
+      <c r="T13" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1971,8 +2122,8 @@
       <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>196</v>
+      <c r="F14" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G14" s="3">
         <v>4</v>
@@ -1989,12 +2140,8 @@
       <c r="K14" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="5" t="s">
         <v>196</v>
       </c>
@@ -2013,9 +2160,15 @@
       <c r="S14" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="2" t="s">
+      <c r="T14" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2030,8 +2183,8 @@
       <c r="E15" s="3">
         <v>1</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>196</v>
+      <c r="F15" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G15" s="3">
         <v>3</v>
@@ -2048,12 +2201,8 @@
       <c r="K15" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="5" t="s">
         <v>196</v>
       </c>
@@ -2072,9 +2221,15 @@
       <c r="S15" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="2" t="s">
+      <c r="T15" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2089,8 +2244,8 @@
       <c r="E16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>196</v>
+      <c r="F16" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G16" s="3">
         <v>3</v>
@@ -2107,12 +2262,8 @@
       <c r="K16" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="5" t="s">
         <v>196</v>
       </c>
@@ -2131,9 +2282,15 @@
       <c r="S16" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="2" t="s">
+      <c r="T16" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2148,8 +2305,8 @@
       <c r="E17" s="3">
         <v>1</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>196</v>
+      <c r="F17" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G17" s="3">
         <v>5</v>
@@ -2166,12 +2323,8 @@
       <c r="K17" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
       <c r="N17" s="5" t="s">
         <v>196</v>
       </c>
@@ -2190,9 +2343,15 @@
       <c r="S17" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" s="2" t="s">
+      <c r="T17" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2207,8 +2366,8 @@
       <c r="E18" s="3">
         <v>1</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>196</v>
+      <c r="F18" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G18" s="3">
         <v>3</v>
@@ -2225,12 +2384,8 @@
       <c r="K18" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="5" t="s">
         <v>196</v>
       </c>
@@ -2249,9 +2404,15 @@
       <c r="S18" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="2" t="s">
+      <c r="T18" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2266,8 +2427,8 @@
       <c r="E19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>196</v>
+      <c r="F19" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G19" s="3">
         <v>8</v>
@@ -2284,12 +2445,8 @@
       <c r="K19" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
       <c r="N19" s="5" t="s">
         <v>196</v>
       </c>
@@ -2308,9 +2465,15 @@
       <c r="S19" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="2" t="s">
+      <c r="T19" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2325,8 +2488,8 @@
       <c r="E20" s="3">
         <v>1</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>196</v>
+      <c r="F20" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G20" s="3">
         <v>3</v>
@@ -2343,12 +2506,8 @@
       <c r="K20" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="5" t="s">
         <v>196</v>
       </c>
@@ -2367,9 +2526,15 @@
       <c r="S20" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="2" t="s">
+      <c r="T20" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U20" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2384,8 +2549,8 @@
       <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>196</v>
+      <c r="F21" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G21" s="3">
         <v>9</v>
@@ -2402,12 +2567,8 @@
       <c r="K21" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="5" t="s">
         <v>196</v>
       </c>
@@ -2426,9 +2587,15 @@
       <c r="S21" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="2" t="s">
+      <c r="T21" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U21" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2443,8 +2610,8 @@
       <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>196</v>
+      <c r="F22" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G22" s="3">
         <v>9</v>
@@ -2461,12 +2628,8 @@
       <c r="K22" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="5" t="s">
         <v>196</v>
       </c>
@@ -2485,9 +2648,15 @@
       <c r="S22" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="2" t="s">
+      <c r="T22" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U22" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2502,8 +2671,8 @@
       <c r="E23" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>196</v>
+      <c r="F23" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G23" s="3">
         <v>3</v>
@@ -2520,12 +2689,8 @@
       <c r="K23" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="5" t="s">
         <v>196</v>
       </c>
@@ -2544,9 +2709,15 @@
       <c r="S23" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="2" t="s">
+      <c r="T23" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2561,8 +2732,8 @@
       <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>196</v>
+      <c r="F24" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G24" s="3">
         <v>3</v>
@@ -2579,12 +2750,8 @@
       <c r="K24" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="5" t="s">
         <v>196</v>
       </c>
@@ -2603,9 +2770,15 @@
       <c r="S24" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="2" t="s">
+      <c r="T24" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U24" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2620,8 +2793,8 @@
       <c r="E25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>196</v>
+      <c r="F25" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G25" s="3">
         <v>3</v>
@@ -2638,12 +2811,8 @@
       <c r="K25" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="5" t="s">
         <v>196</v>
       </c>
@@ -2662,9 +2831,15 @@
       <c r="S25" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="2" t="s">
+      <c r="T25" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U25" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2679,8 +2854,8 @@
       <c r="E26" s="3">
         <v>1</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>196</v>
+      <c r="F26" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G26" s="3">
         <v>3</v>
@@ -2697,12 +2872,8 @@
       <c r="K26" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
       <c r="N26" s="5" t="s">
         <v>196</v>
       </c>
@@ -2721,9 +2892,15 @@
       <c r="S26" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="27" spans="1:19">
-      <c r="A27" s="2" t="s">
+      <c r="T26" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U26" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2738,8 +2915,8 @@
       <c r="E27" s="3">
         <v>1</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>196</v>
+      <c r="F27" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G27" s="3">
         <v>3</v>
@@ -2756,12 +2933,8 @@
       <c r="K27" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
       <c r="N27" s="5" t="s">
         <v>196</v>
       </c>
@@ -2780,9 +2953,15 @@
       <c r="S27" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="28" spans="1:19">
-      <c r="A28" s="2" t="s">
+      <c r="T27" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U27" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2797,8 +2976,8 @@
       <c r="E28" s="3">
         <v>1</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>196</v>
+      <c r="F28" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G28" s="3">
         <v>3</v>
@@ -2815,12 +2994,8 @@
       <c r="K28" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
       <c r="N28" s="5" t="s">
         <v>196</v>
       </c>
@@ -2839,9 +3014,15 @@
       <c r="S28" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29" s="2" t="s">
+      <c r="T28" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2856,8 +3037,8 @@
       <c r="E29" s="3">
         <v>1</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>196</v>
+      <c r="F29" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G29" s="3">
         <v>3</v>
@@ -2874,12 +3055,8 @@
       <c r="K29" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
       <c r="N29" s="5" t="s">
         <v>196</v>
       </c>
@@ -2898,9 +3075,15 @@
       <c r="S29" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="30" spans="1:19">
-      <c r="A30" s="2" t="s">
+      <c r="T29" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U29" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -2915,8 +3098,8 @@
       <c r="E30" s="3">
         <v>1</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>196</v>
+      <c r="F30" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G30" s="3">
         <v>3</v>
@@ -2933,12 +3116,8 @@
       <c r="K30" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
       <c r="N30" s="5" t="s">
         <v>196</v>
       </c>
@@ -2957,9 +3136,15 @@
       <c r="S30" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="31" spans="1:19">
-      <c r="A31" s="2" t="s">
+      <c r="T30" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U30" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2974,8 +3159,8 @@
       <c r="E31" s="3">
         <v>1</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>196</v>
+      <c r="F31" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G31" s="3">
         <v>8</v>
@@ -2992,12 +3177,8 @@
       <c r="K31" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
       <c r="N31" s="5" t="s">
         <v>196</v>
       </c>
@@ -3016,9 +3197,15 @@
       <c r="S31" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="32" spans="1:19">
-      <c r="A32" s="2" t="s">
+      <c r="T31" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U31" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3033,8 +3220,8 @@
       <c r="E32" s="3">
         <v>1</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>196</v>
+      <c r="F32" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G32" s="3">
         <v>5</v>
@@ -3051,12 +3238,8 @@
       <c r="K32" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L32" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
       <c r="N32" s="5" t="s">
         <v>196</v>
       </c>
@@ -3075,9 +3258,15 @@
       <c r="S32" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="33" spans="1:19">
-      <c r="A33" s="2" t="s">
+      <c r="T32" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U32" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3092,8 +3281,8 @@
       <c r="E33" s="3">
         <v>1</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>196</v>
+      <c r="F33" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G33" s="3">
         <v>5</v>
@@ -3110,12 +3299,8 @@
       <c r="K33" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
       <c r="N33" s="5" t="s">
         <v>196</v>
       </c>
@@ -3134,9 +3319,15 @@
       <c r="S33" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="34" spans="1:19">
-      <c r="A34" s="2" t="s">
+      <c r="T33" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U33" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -3151,8 +3342,8 @@
       <c r="E34" s="3">
         <v>1</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>196</v>
+      <c r="F34" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G34" s="3">
         <v>5</v>
@@ -3169,12 +3360,8 @@
       <c r="K34" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L34" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
       <c r="N34" s="5" t="s">
         <v>196</v>
       </c>
@@ -3193,9 +3380,15 @@
       <c r="S34" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="35" spans="1:19">
-      <c r="A35" s="2" t="s">
+      <c r="T34" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U34" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -3210,8 +3403,8 @@
       <c r="E35" s="3">
         <v>1</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>196</v>
+      <c r="F35" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G35" s="3">
         <v>4</v>
@@ -3228,12 +3421,8 @@
       <c r="K35" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L35" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
       <c r="N35" s="5" t="s">
         <v>196</v>
       </c>
@@ -3252,9 +3441,15 @@
       <c r="S35" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="36" spans="1:19">
-      <c r="A36" s="2" t="s">
+      <c r="T35" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U35" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3269,8 +3464,8 @@
       <c r="E36" s="3">
         <v>1</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>196</v>
+      <c r="F36" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G36" s="3">
         <v>4</v>
@@ -3287,12 +3482,8 @@
       <c r="K36" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L36" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
       <c r="N36" s="5" t="s">
         <v>196</v>
       </c>
@@ -3311,9 +3502,15 @@
       <c r="S36" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="37" spans="1:19">
-      <c r="A37" s="2" t="s">
+      <c r="T36" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -3328,8 +3525,8 @@
       <c r="E37" s="3">
         <v>1</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>196</v>
+      <c r="F37" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G37" s="3">
         <v>6</v>
@@ -3346,12 +3543,8 @@
       <c r="K37" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L37" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
       <c r="N37" s="5" t="s">
         <v>196</v>
       </c>
@@ -3370,9 +3563,15 @@
       <c r="S37" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="38" spans="1:19">
-      <c r="A38" s="2" t="s">
+      <c r="T37" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U37" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -3387,8 +3586,8 @@
       <c r="E38" s="3">
         <v>2</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>196</v>
+      <c r="F38" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G38" s="3">
         <v>100</v>
@@ -3405,12 +3604,8 @@
       <c r="K38" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L38" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
       <c r="N38" s="5" t="s">
         <v>196</v>
       </c>
@@ -3429,9 +3624,15 @@
       <c r="S38" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="39" spans="1:19">
-      <c r="A39" s="2" t="s">
+      <c r="T38" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U38" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -3446,8 +3647,8 @@
       <c r="E39" s="3">
         <v>1</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>196</v>
+      <c r="F39" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G39" s="3">
         <v>2</v>
@@ -3464,12 +3665,8 @@
       <c r="K39" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L39" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
       <c r="N39" s="5" t="s">
         <v>196</v>
       </c>
@@ -3488,9 +3685,15 @@
       <c r="S39" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="40" spans="1:19">
-      <c r="A40" s="2" t="s">
+      <c r="T39" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U39" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -3505,8 +3708,8 @@
       <c r="E40" s="3">
         <v>2</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>196</v>
+      <c r="F40" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G40" s="3">
         <v>30</v>
@@ -3523,12 +3726,8 @@
       <c r="K40" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L40" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
       <c r="N40" s="5" t="s">
         <v>196</v>
       </c>
@@ -3547,9 +3746,15 @@
       <c r="S40" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="41" spans="1:19">
-      <c r="A41" s="2" t="s">
+      <c r="T40" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U40" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -3564,8 +3769,8 @@
       <c r="E41" s="3">
         <v>8</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>196</v>
+      <c r="F41" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G41" s="3">
         <v>1</v>
@@ -3579,12 +3784,8 @@
       <c r="K41" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L41" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
       <c r="N41" s="5" t="s">
         <v>196</v>
       </c>
@@ -3603,9 +3804,15 @@
       <c r="S41" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="42" spans="1:19">
-      <c r="A42" s="2" t="s">
+      <c r="T41" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U41" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="A42" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -3620,8 +3827,8 @@
       <c r="E42" s="3">
         <v>2</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>196</v>
+      <c r="F42" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G42" s="3">
         <v>30</v>
@@ -3638,12 +3845,8 @@
       <c r="K42" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L42" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
       <c r="N42" s="5" t="s">
         <v>196</v>
       </c>
@@ -3662,9 +3865,15 @@
       <c r="S42" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="43" spans="1:19">
-      <c r="A43" s="2" t="s">
+      <c r="T42" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U42" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -3679,8 +3888,8 @@
       <c r="E43" s="3">
         <v>1</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>196</v>
+      <c r="F43" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G43" s="3">
         <v>2</v>
@@ -3697,12 +3906,8 @@
       <c r="K43" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L43" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M43" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
       <c r="N43" s="5" t="s">
         <v>196</v>
       </c>
@@ -3721,9 +3926,15 @@
       <c r="S43" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="44" spans="1:19">
-      <c r="A44" s="2" t="s">
+      <c r="T43" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U43" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -3738,8 +3949,8 @@
       <c r="E44" s="3">
         <v>2</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>196</v>
+      <c r="F44" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G44" s="3">
         <v>99</v>
@@ -3756,12 +3967,8 @@
       <c r="K44" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L44" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M44" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
       <c r="N44" s="5" t="s">
         <v>196</v>
       </c>
@@ -3780,9 +3987,15 @@
       <c r="S44" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="45" spans="1:19">
-      <c r="A45" s="2" t="s">
+      <c r="T44" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U44" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3797,8 +4010,8 @@
       <c r="E45" s="3">
         <v>1</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>196</v>
+      <c r="F45" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G45" s="3">
         <v>3</v>
@@ -3815,12 +4028,8 @@
       <c r="K45" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L45" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M45" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
       <c r="N45" s="5" t="s">
         <v>196</v>
       </c>
@@ -3839,9 +4048,15 @@
       <c r="S45" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="46" spans="1:19">
-      <c r="A46" s="2" t="s">
+      <c r="T45" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U45" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
+      <c r="A46" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -3856,8 +4071,8 @@
       <c r="E46" s="3">
         <v>2</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>196</v>
+      <c r="F46" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G46" s="3">
         <v>12</v>
@@ -3874,12 +4089,8 @@
       <c r="K46" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L46" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M46" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
       <c r="N46" s="5" t="s">
         <v>196</v>
       </c>
@@ -3898,9 +4109,15 @@
       <c r="S46" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="47" spans="1:19">
-      <c r="A47" s="2" t="s">
+      <c r="T46" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U46" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="A47" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -3915,8 +4132,8 @@
       <c r="E47" s="3">
         <v>1</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>196</v>
+      <c r="F47" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G47" s="3">
         <v>2</v>
@@ -3933,12 +4150,8 @@
       <c r="K47" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L47" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M47" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
       <c r="N47" s="5" t="s">
         <v>196</v>
       </c>
@@ -3957,9 +4170,15 @@
       <c r="S47" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="48" spans="1:19">
-      <c r="A48" s="2" t="s">
+      <c r="T47" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U47" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="A48" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -3974,8 +4193,8 @@
       <c r="E48" s="3">
         <v>1</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>196</v>
+      <c r="F48" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G48" s="3">
         <v>2</v>
@@ -3992,12 +4211,8 @@
       <c r="K48" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L48" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M48" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
       <c r="N48" s="5" t="s">
         <v>196</v>
       </c>
@@ -4016,9 +4231,15 @@
       <c r="S48" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="49" spans="1:19">
-      <c r="A49" s="2" t="s">
+      <c r="T48" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U48" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="A49" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -4033,8 +4254,8 @@
       <c r="E49" s="3">
         <v>1</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>196</v>
+      <c r="F49" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G49" s="3">
         <v>2</v>
@@ -4051,12 +4272,8 @@
       <c r="K49" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L49" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M49" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
       <c r="N49" s="5" t="s">
         <v>196</v>
       </c>
@@ -4075,9 +4292,15 @@
       <c r="S49" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="50" spans="1:19">
-      <c r="A50" s="2" t="s">
+      <c r="T49" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U49" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -4092,8 +4315,8 @@
       <c r="E50" s="3">
         <v>1</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>196</v>
+      <c r="F50" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G50" s="3">
         <v>2</v>
@@ -4110,12 +4333,8 @@
       <c r="K50" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L50" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M50" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
       <c r="N50" s="5" t="s">
         <v>196</v>
       </c>
@@ -4134,9 +4353,15 @@
       <c r="S50" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="51" spans="1:19">
-      <c r="A51" s="2" t="s">
+      <c r="T50" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U50" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
+      <c r="A51" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -4151,8 +4376,8 @@
       <c r="E51" s="3">
         <v>1</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>196</v>
+      <c r="F51" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G51" s="3">
         <v>2</v>
@@ -4169,12 +4394,8 @@
       <c r="K51" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L51" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M51" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
       <c r="N51" s="5" t="s">
         <v>196</v>
       </c>
@@ -4193,9 +4414,15 @@
       <c r="S51" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="52" spans="1:19">
-      <c r="A52" s="2" t="s">
+      <c r="T51" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U51" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="A52" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -4210,8 +4437,8 @@
       <c r="E52" s="3">
         <v>1</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>196</v>
+      <c r="F52" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G52" s="3">
         <v>2</v>
@@ -4228,12 +4455,8 @@
       <c r="K52" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L52" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
       <c r="N52" s="5" t="s">
         <v>196</v>
       </c>
@@ -4252,9 +4475,15 @@
       <c r="S52" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="A53" s="2" t="s">
+      <c r="T52" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U52" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -4269,8 +4498,8 @@
       <c r="E53" s="3">
         <v>1</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>196</v>
+      <c r="F53" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G53" s="3">
         <v>2</v>
@@ -4287,12 +4516,8 @@
       <c r="K53" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L53" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M53" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
       <c r="N53" s="5" t="s">
         <v>196</v>
       </c>
@@ -4311,9 +4536,15 @@
       <c r="S53" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="54" spans="1:19">
-      <c r="A54" s="2" t="s">
+      <c r="T53" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U53" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21">
+      <c r="A54" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -4328,8 +4559,8 @@
       <c r="E54" s="3">
         <v>1</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>196</v>
+      <c r="F54" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G54" s="3">
         <v>3</v>
@@ -4346,12 +4577,8 @@
       <c r="K54" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L54" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M54" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
       <c r="N54" s="5" t="s">
         <v>196</v>
       </c>
@@ -4370,9 +4597,15 @@
       <c r="S54" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="55" spans="1:19">
-      <c r="A55" s="2" t="s">
+      <c r="T54" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U54" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21">
+      <c r="A55" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -4387,8 +4620,8 @@
       <c r="E55" s="3">
         <v>3</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>196</v>
+      <c r="F55" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G55" s="3">
         <v>14</v>
@@ -4405,12 +4638,8 @@
       <c r="K55" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L55" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M55" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
       <c r="N55" s="5" t="s">
         <v>196</v>
       </c>
@@ -4429,9 +4658,15 @@
       <c r="S55" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="56" spans="1:19">
-      <c r="A56" s="2" t="s">
+      <c r="T55" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U55" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="A56" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -4446,8 +4681,8 @@
       <c r="E56" s="3">
         <v>2</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>196</v>
+      <c r="F56" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G56" s="3">
         <v>11</v>
@@ -4464,12 +4699,8 @@
       <c r="K56" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L56" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
       <c r="N56" s="5" t="s">
         <v>196</v>
       </c>
@@ -4488,9 +4719,15 @@
       <c r="S56" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="57" spans="1:19">
-      <c r="A57" s="2" t="s">
+      <c r="T56" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U56" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21">
+      <c r="A57" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -4505,8 +4742,8 @@
       <c r="E57" s="3">
         <v>4</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>196</v>
+      <c r="F57" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G57" s="3">
         <v>111</v>
@@ -4523,12 +4760,8 @@
       <c r="K57" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L57" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M57" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
       <c r="N57" s="5" t="s">
         <v>196</v>
       </c>
@@ -4547,9 +4780,15 @@
       <c r="S57" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="A58" s="2" t="s">
+      <c r="T57" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U57" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21">
+      <c r="A58" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -4564,8 +4803,8 @@
       <c r="E58" s="3">
         <v>1</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>196</v>
+      <c r="F58" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G58" s="3">
         <v>3</v>
@@ -4582,12 +4821,8 @@
       <c r="K58" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L58" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M58" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
       <c r="N58" s="5" t="s">
         <v>196</v>
       </c>
@@ -4606,9 +4841,15 @@
       <c r="S58" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="59" spans="1:19">
-      <c r="A59" s="2" t="s">
+      <c r="T58" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U58" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21">
+      <c r="A59" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -4623,8 +4864,8 @@
       <c r="E59" s="3">
         <v>3</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>196</v>
+      <c r="F59" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G59" s="3">
         <v>33</v>
@@ -4641,12 +4882,8 @@
       <c r="K59" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L59" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M59" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
       <c r="N59" s="5" t="s">
         <v>196</v>
       </c>
@@ -4665,9 +4902,15 @@
       <c r="S59" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="60" spans="1:19">
-      <c r="A60" s="2" t="s">
+      <c r="T59" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U59" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21">
+      <c r="A60" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -4682,8 +4925,8 @@
       <c r="E60" s="3">
         <v>4</v>
       </c>
-      <c r="F60" s="2" t="s">
-        <v>196</v>
+      <c r="F60" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G60" s="3">
         <v>47</v>
@@ -4700,12 +4943,8 @@
       <c r="K60" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L60" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
       <c r="N60" s="5" t="s">
         <v>196</v>
       </c>
@@ -4724,9 +4963,15 @@
       <c r="S60" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="61" spans="1:19">
-      <c r="A61" s="2" t="s">
+      <c r="T60" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U60" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
+      <c r="A61" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -4741,8 +4986,8 @@
       <c r="E61" s="3">
         <v>2</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>196</v>
+      <c r="F61" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G61" s="3">
         <v>11</v>
@@ -4759,12 +5004,8 @@
       <c r="K61" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L61" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M61" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
       <c r="N61" s="5" t="s">
         <v>196</v>
       </c>
@@ -4783,9 +5024,15 @@
       <c r="S61" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="62" spans="1:19">
-      <c r="A62" s="2" t="s">
+      <c r="T61" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U61" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21">
+      <c r="A62" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -4800,8 +5047,8 @@
       <c r="E62" s="3">
         <v>4</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>196</v>
+      <c r="F62" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G62" s="3">
         <v>123</v>
@@ -4818,12 +5065,8 @@
       <c r="K62" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L62" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M62" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
       <c r="N62" s="5" t="s">
         <v>196</v>
       </c>
@@ -4842,16 +5085,22 @@
       <c r="S62" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="63" spans="1:19">
-      <c r="A63" s="2" t="s">
+      <c r="T62" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U62" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21">
+      <c r="A63" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>196</v>
+      <c r="C63" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>198</v>
@@ -4859,8 +5108,8 @@
       <c r="E63" s="3">
         <v>1</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>196</v>
+      <c r="F63" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G63" s="3">
         <v>8</v>
@@ -4877,12 +5126,8 @@
       <c r="K63" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L63" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M63" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
       <c r="N63" s="5" t="s">
         <v>196</v>
       </c>
@@ -4901,16 +5146,22 @@
       <c r="S63" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="64" spans="1:19">
-      <c r="A64" s="2" t="s">
+      <c r="T63" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U63" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="A64" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>196</v>
+      <c r="C64" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>198</v>
@@ -4918,8 +5169,8 @@
       <c r="E64" s="3">
         <v>1</v>
       </c>
-      <c r="F64" s="2" t="s">
-        <v>196</v>
+      <c r="F64" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G64" s="3">
         <v>4</v>
@@ -4936,12 +5187,8 @@
       <c r="K64" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L64" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M64" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
       <c r="N64" s="5" t="s">
         <v>196</v>
       </c>
@@ -4960,16 +5207,22 @@
       <c r="S64" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="65" spans="1:19">
-      <c r="A65" s="2" t="s">
+      <c r="T64" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U64" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21">
+      <c r="A65" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>196</v>
+      <c r="C65" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>198</v>
@@ -4977,8 +5230,8 @@
       <c r="E65" s="3">
         <v>1</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>196</v>
+      <c r="F65" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G65" s="3">
         <v>5</v>
@@ -4995,12 +5248,8 @@
       <c r="K65" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L65" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M65" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
       <c r="N65" s="5" t="s">
         <v>196</v>
       </c>
@@ -5019,16 +5268,22 @@
       <c r="S65" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="66" spans="1:19">
-      <c r="A66" s="2" t="s">
+      <c r="T65" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U65" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21">
+      <c r="A66" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>196</v>
+      <c r="C66" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>198</v>
@@ -5036,8 +5291,8 @@
       <c r="E66" s="3">
         <v>1</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>196</v>
+      <c r="F66" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G66" s="3">
         <v>5</v>
@@ -5051,26 +5306,24 @@
       <c r="J66" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="K66" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="L66" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M66" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N66" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O66" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P66" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q66" s="5" t="s">
-        <v>196</v>
+      <c r="K66" s="5">
+        <v>0</v>
+      </c>
+      <c r="L66" s="5">
+        <v>1</v>
+      </c>
+      <c r="M66" s="5"/>
+      <c r="N66" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O66" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="P66" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q66" s="9" t="s">
+        <v>261</v>
       </c>
       <c r="R66" s="5" t="s">
         <v>196</v>
@@ -5078,16 +5331,22 @@
       <c r="S66" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="67" spans="1:19">
-      <c r="A67" s="2" t="s">
+      <c r="T66" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U66" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21">
+      <c r="A67" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>196</v>
+      <c r="C67" s="7" t="s">
+        <v>262</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>198</v>
@@ -5095,8 +5354,8 @@
       <c r="E67" s="3">
         <v>2</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>196</v>
+      <c r="F67" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G67" s="3">
         <v>15</v>
@@ -5113,17 +5372,15 @@
       <c r="K67" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L67" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M67" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N67" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O67" s="5" t="s">
-        <v>196</v>
+      <c r="L67" s="5">
+        <v>1</v>
+      </c>
+      <c r="M67" s="5"/>
+      <c r="N67" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O67" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="P67" s="5" t="s">
         <v>196</v>
@@ -5137,16 +5394,22 @@
       <c r="S67" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="68" spans="1:19">
-      <c r="A68" s="2" t="s">
+      <c r="T67" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U67" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21">
+      <c r="A68" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>196</v>
+      <c r="C68" s="7" t="s">
+        <v>263</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>198</v>
@@ -5154,8 +5417,8 @@
       <c r="E68" s="3">
         <v>2</v>
       </c>
-      <c r="F68" s="2" t="s">
-        <v>196</v>
+      <c r="F68" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G68" s="3">
         <v>10</v>
@@ -5172,17 +5435,15 @@
       <c r="K68" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L68" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M68" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N68" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O68" s="5" t="s">
-        <v>196</v>
+      <c r="L68" s="5">
+        <v>1</v>
+      </c>
+      <c r="M68" s="5"/>
+      <c r="N68" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O68" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>196</v>
@@ -5196,16 +5457,22 @@
       <c r="S68" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="69" spans="1:19">
-      <c r="A69" s="2" t="s">
+      <c r="T68" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U68" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21">
+      <c r="A69" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>196</v>
+      <c r="C69" s="7" t="s">
+        <v>264</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>198</v>
@@ -5213,8 +5480,8 @@
       <c r="E69" s="3">
         <v>3</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>196</v>
+      <c r="F69" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G69" s="3">
         <v>55</v>
@@ -5231,17 +5498,15 @@
       <c r="K69" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L69" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O69" s="5" t="s">
-        <v>196</v>
+      <c r="L69" s="5">
+        <v>1</v>
+      </c>
+      <c r="M69" s="5"/>
+      <c r="N69" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O69" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>196</v>
@@ -5255,16 +5520,22 @@
       <c r="S69" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="70" spans="1:19">
-      <c r="A70" s="2" t="s">
+      <c r="T69" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U69" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21">
+      <c r="A70" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>196</v>
+      <c r="C70" s="7" t="s">
+        <v>266</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>198</v>
@@ -5272,8 +5543,8 @@
       <c r="E70" s="3">
         <v>2</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>196</v>
+      <c r="F70" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G70" s="3">
         <v>8</v>
@@ -5290,23 +5561,21 @@
       <c r="K70" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L70" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M70" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O70" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P70" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q70" s="5" t="s">
-        <v>196</v>
+      <c r="L70" s="5">
+        <v>2</v>
+      </c>
+      <c r="M70" s="5"/>
+      <c r="N70" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O70" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="P70" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q70" s="9" t="s">
+        <v>268</v>
       </c>
       <c r="R70" s="5" t="s">
         <v>196</v>
@@ -5314,16 +5583,22 @@
       <c r="S70" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="71" spans="1:19">
-      <c r="A71" s="2" t="s">
+      <c r="T70" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U70" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21">
+      <c r="A71" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>196</v>
+      <c r="C71" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>198</v>
@@ -5331,8 +5606,8 @@
       <c r="E71" s="3">
         <v>2</v>
       </c>
-      <c r="F71" s="2" t="s">
-        <v>196</v>
+      <c r="F71" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G71" s="3">
         <v>10</v>
@@ -5349,23 +5624,21 @@
       <c r="K71" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L71" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M71" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N71" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O71" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P71" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q71" s="5" t="s">
-        <v>196</v>
+      <c r="L71" s="5">
+        <v>2</v>
+      </c>
+      <c r="M71" s="5"/>
+      <c r="N71" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O71" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="P71" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q71" s="9" t="s">
+        <v>268</v>
       </c>
       <c r="R71" s="5" t="s">
         <v>196</v>
@@ -5373,16 +5646,22 @@
       <c r="S71" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="72" spans="1:19">
-      <c r="A72" s="2" t="s">
+      <c r="T71" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U71" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21">
+      <c r="A72" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>196</v>
+      <c r="C72" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>198</v>
@@ -5390,8 +5669,8 @@
       <c r="E72" s="3">
         <v>1</v>
       </c>
-      <c r="F72" s="2" t="s">
-        <v>196</v>
+      <c r="F72" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G72" s="3">
         <v>4</v>
@@ -5408,12 +5687,8 @@
       <c r="K72" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L72" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M72" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
       <c r="N72" s="5" t="s">
         <v>196</v>
       </c>
@@ -5432,16 +5707,22 @@
       <c r="S72" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="73" spans="1:19">
-      <c r="A73" s="2" t="s">
+      <c r="T72" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U72" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21">
+      <c r="A73" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>196</v>
+      <c r="C73" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>198</v>
@@ -5449,8 +5730,8 @@
       <c r="E73" s="3">
         <v>3</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>196</v>
+      <c r="F73" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G73" s="3">
         <v>24</v>
@@ -5467,12 +5748,8 @@
       <c r="K73" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L73" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M73" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
       <c r="N73" s="5" t="s">
         <v>196</v>
       </c>
@@ -5491,16 +5768,22 @@
       <c r="S73" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="74" spans="1:19">
-      <c r="A74" s="2" t="s">
+      <c r="T73" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U73" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21">
+      <c r="A74" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>196</v>
+      <c r="C74" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>198</v>
@@ -5508,8 +5791,8 @@
       <c r="E74" s="3">
         <v>2</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>196</v>
+      <c r="F74" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G74" s="3">
         <v>11</v>
@@ -5526,12 +5809,8 @@
       <c r="K74" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L74" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M74" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
       <c r="N74" s="5" t="s">
         <v>196</v>
       </c>
@@ -5550,16 +5829,22 @@
       <c r="S74" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="75" spans="1:19">
-      <c r="A75" s="2" t="s">
+      <c r="T74" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U74" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21">
+      <c r="A75" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>196</v>
+      <c r="C75" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>198</v>
@@ -5567,8 +5852,8 @@
       <c r="E75" s="3">
         <v>4</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>196</v>
+      <c r="F75" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G75" s="3">
         <v>123</v>
@@ -5585,12 +5870,8 @@
       <c r="K75" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L75" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M75" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
       <c r="N75" s="5" t="s">
         <v>196</v>
       </c>
@@ -5609,16 +5890,22 @@
       <c r="S75" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="76" spans="1:19">
-      <c r="A76" s="2" t="s">
+      <c r="T75" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U75" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21">
+      <c r="A76" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>196</v>
+      <c r="C76" s="7" t="s">
+        <v>269</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>198</v>
@@ -5626,8 +5913,8 @@
       <c r="E76" s="3">
         <v>1</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>196</v>
+      <c r="F76" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G76" s="3">
         <v>4</v>
@@ -5644,17 +5931,15 @@
       <c r="K76" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L76" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M76" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N76" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O76" s="5" t="s">
-        <v>196</v>
+      <c r="L76" s="5">
+        <v>1</v>
+      </c>
+      <c r="M76" s="5"/>
+      <c r="N76" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O76" s="9" t="s">
+        <v>270</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>196</v>
@@ -5668,16 +5953,22 @@
       <c r="S76" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="77" spans="1:19">
-      <c r="A77" s="2" t="s">
+      <c r="T76" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U76" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21">
+      <c r="A77" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>196</v>
+      <c r="C77" s="7" t="s">
+        <v>271</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>198</v>
@@ -5685,8 +5976,8 @@
       <c r="E77" s="3">
         <v>1</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>196</v>
+      <c r="F77" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G77" s="3">
         <v>7</v>
@@ -5703,23 +5994,21 @@
       <c r="K77" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L77" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M77" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N77" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O77" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P77" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q77" s="5" t="s">
-        <v>196</v>
+      <c r="L77" s="5">
+        <v>2</v>
+      </c>
+      <c r="M77" s="5"/>
+      <c r="N77" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O77" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="P77" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q77" s="5">
+        <v>2</v>
       </c>
       <c r="R77" s="5" t="s">
         <v>196</v>
@@ -5727,16 +6016,22 @@
       <c r="S77" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="78" spans="1:19">
-      <c r="A78" s="2" t="s">
+      <c r="T77" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U77" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21">
+      <c r="A78" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>196</v>
+      <c r="C78" s="7" t="s">
+        <v>272</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>198</v>
@@ -5744,8 +6039,8 @@
       <c r="E78" s="3">
         <v>1</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>196</v>
+      <c r="F78" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G78" s="3">
         <v>8</v>
@@ -5762,40 +6057,44 @@
       <c r="K78" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L78" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M78" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N78" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O78" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P78" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q78" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="R78" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="S78" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19">
-      <c r="A79" s="2" t="s">
+      <c r="L78" s="5">
+        <v>3</v>
+      </c>
+      <c r="M78" s="5"/>
+      <c r="N78" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O78" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="P78" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q78" s="5">
+        <v>2</v>
+      </c>
+      <c r="R78" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="S78" s="5">
+        <v>5</v>
+      </c>
+      <c r="T78" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U78" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21">
+      <c r="A79" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>196</v>
+      <c r="C79" s="7" t="s">
+        <v>273</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>198</v>
@@ -5803,8 +6102,8 @@
       <c r="E79" s="3">
         <v>3</v>
       </c>
-      <c r="F79" s="2" t="s">
-        <v>196</v>
+      <c r="F79" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G79" s="3">
         <v>124</v>
@@ -5821,40 +6120,39 @@
       <c r="K79" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L79" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M79" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N79" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O79" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P79" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q79" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L79" s="5">
+        <v>3</v>
+      </c>
+      <c r="M79" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="N79" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O79" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="5"/>
       <c r="R79" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S79" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19">
-      <c r="A80" s="2" t="s">
+      <c r="T79" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="U79" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21">
+      <c r="A80" s="5" t="s">
         <v>97</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>196</v>
+      <c r="C80" s="7" t="s">
+        <v>274</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>198</v>
@@ -5862,8 +6160,8 @@
       <c r="E80" s="3">
         <v>1</v>
       </c>
-      <c r="F80" s="2" t="s">
-        <v>196</v>
+      <c r="F80" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G80" s="3">
         <v>7</v>
@@ -5880,40 +6178,39 @@
       <c r="K80" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L80" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M80" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N80" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O80" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P80" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q80" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L80" s="5">
+        <v>3</v>
+      </c>
+      <c r="M80" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="N80" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O80" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="5"/>
       <c r="R80" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S80" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="81" spans="1:19">
-      <c r="A81" s="2" t="s">
+      <c r="T80" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="U80" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21">
+      <c r="A81" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>196</v>
+      <c r="C81" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>198</v>
@@ -5921,8 +6218,8 @@
       <c r="E81" s="3">
         <v>3</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>196</v>
+      <c r="F81" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G81" s="3">
         <v>132</v>
@@ -5939,40 +6236,39 @@
       <c r="K81" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L81" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M81" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N81" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O81" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P81" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q81" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L81" s="5">
+        <v>3</v>
+      </c>
+      <c r="M81" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="N81" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O81" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="P81" s="2"/>
+      <c r="Q81" s="5"/>
       <c r="R81" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="S81" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="82" spans="1:19">
-      <c r="A82" s="2" t="s">
+      <c r="T81" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="U81" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21">
+      <c r="A82" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>196</v>
+      <c r="C82" s="7" t="s">
+        <v>276</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>198</v>
@@ -5980,8 +6276,8 @@
       <c r="E82" s="3">
         <v>1</v>
       </c>
-      <c r="F82" s="2" t="s">
-        <v>196</v>
+      <c r="F82" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G82" s="3">
         <v>7</v>
@@ -5998,40 +6294,40 @@
       <c r="K82" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L82" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M82" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N82" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O82" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P82" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q82" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="L82" s="5">
+        <v>1</v>
+      </c>
+      <c r="M82" s="5"/>
+      <c r="N82" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O82" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="5"/>
       <c r="R82" s="5" t="s">
         <v>196</v>
       </c>
       <c r="S82" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="83" spans="1:19">
-      <c r="A83" s="2" t="s">
+      <c r="T82" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U82" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21">
+      <c r="A83" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>196</v>
+      <c r="C83" s="7" t="s">
+        <v>277</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>198</v>
@@ -6039,8 +6335,8 @@
       <c r="E83" s="3">
         <v>1</v>
       </c>
-      <c r="F83" s="2" t="s">
-        <v>196</v>
+      <c r="F83" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G83" s="3">
         <v>8</v>
@@ -6057,17 +6353,15 @@
       <c r="K83" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L83" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M83" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N83" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O83" s="5" t="s">
-        <v>196</v>
+      <c r="L83" s="5">
+        <v>1</v>
+      </c>
+      <c r="M83" s="5"/>
+      <c r="N83" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O83" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="P83" s="5" t="s">
         <v>196</v>
@@ -6081,16 +6375,22 @@
       <c r="S83" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="84" spans="1:19">
-      <c r="A84" s="2" t="s">
+      <c r="T83" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U83" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21">
+      <c r="A84" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>196</v>
+      <c r="C84" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>198</v>
@@ -6098,8 +6398,8 @@
       <c r="E84" s="3">
         <v>2</v>
       </c>
-      <c r="F84" s="2" t="s">
-        <v>196</v>
+      <c r="F84" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G84" s="3">
         <v>21</v>
@@ -6116,23 +6416,21 @@
       <c r="K84" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L84" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M84" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N84" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O84" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P84" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q84" s="5" t="s">
-        <v>196</v>
+      <c r="L84" s="5">
+        <v>2</v>
+      </c>
+      <c r="M84" s="5"/>
+      <c r="N84" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O84" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="P84" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q84" s="5">
+        <v>2</v>
       </c>
       <c r="R84" s="5" t="s">
         <v>196</v>
@@ -6140,16 +6438,22 @@
       <c r="S84" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="85" spans="1:19">
-      <c r="A85" s="2" t="s">
+      <c r="T84" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U84" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21">
+      <c r="A85" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>196</v>
+      <c r="C85" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>198</v>
@@ -6157,8 +6461,8 @@
       <c r="E85" s="3">
         <v>2</v>
       </c>
-      <c r="F85" s="2" t="s">
-        <v>196</v>
+      <c r="F85" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G85" s="3">
         <v>17</v>
@@ -6175,23 +6479,21 @@
       <c r="K85" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L85" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M85" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N85" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O85" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P85" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q85" s="5" t="s">
-        <v>196</v>
+      <c r="L85" s="5">
+        <v>2</v>
+      </c>
+      <c r="M85" s="5"/>
+      <c r="N85" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O85" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="P85" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q85" s="5">
+        <v>2</v>
       </c>
       <c r="R85" s="5" t="s">
         <v>196</v>
@@ -6199,16 +6501,22 @@
       <c r="S85" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="86" spans="1:19">
-      <c r="A86" s="2" t="s">
+      <c r="T85" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U85" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21">
+      <c r="A86" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>196</v>
+      <c r="C86" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>198</v>
@@ -6216,8 +6524,8 @@
       <c r="E86" s="3">
         <v>2</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>196</v>
+      <c r="F86" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G86" s="3">
         <v>15</v>
@@ -6234,23 +6542,21 @@
       <c r="K86" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L86" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M86" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N86" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O86" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P86" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q86" s="5" t="s">
-        <v>196</v>
+      <c r="L86" s="5">
+        <v>2</v>
+      </c>
+      <c r="M86" s="5"/>
+      <c r="N86" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O86" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="P86" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q86" s="5">
+        <v>2</v>
       </c>
       <c r="R86" s="5" t="s">
         <v>196</v>
@@ -6258,16 +6564,22 @@
       <c r="S86" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="87" spans="1:19">
-      <c r="A87" s="2" t="s">
+      <c r="T86" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U86" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21">
+      <c r="A87" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>196</v>
+      <c r="C87" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>198</v>
@@ -6275,8 +6587,8 @@
       <c r="E87" s="3">
         <v>2</v>
       </c>
-      <c r="F87" s="2" t="s">
-        <v>196</v>
+      <c r="F87" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G87" s="3">
         <v>14</v>
@@ -6293,23 +6605,21 @@
       <c r="K87" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L87" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M87" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N87" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O87" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P87" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q87" s="5" t="s">
-        <v>196</v>
+      <c r="L87" s="5">
+        <v>2</v>
+      </c>
+      <c r="M87" s="5"/>
+      <c r="N87" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O87" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="P87" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q87" s="5">
+        <v>2</v>
       </c>
       <c r="R87" s="5" t="s">
         <v>196</v>
@@ -6317,16 +6627,22 @@
       <c r="S87" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="88" spans="1:19">
-      <c r="A88" s="2" t="s">
+      <c r="T87" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U87" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21">
+      <c r="A88" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>196</v>
+      <c r="C88" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>198</v>
@@ -6334,8 +6650,8 @@
       <c r="E88" s="3">
         <v>4</v>
       </c>
-      <c r="F88" s="2" t="s">
-        <v>196</v>
+      <c r="F88" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="G88" s="3">
         <v>64</v>
@@ -6352,23 +6668,21 @@
       <c r="K88" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L88" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M88" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N88" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O88" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P88" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q88" s="5" t="s">
-        <v>196</v>
+      <c r="L88" s="5">
+        <v>2</v>
+      </c>
+      <c r="M88" s="5"/>
+      <c r="N88" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O88" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="P88" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q88" s="5">
+        <v>2</v>
       </c>
       <c r="R88" s="5" t="s">
         <v>196</v>
@@ -6376,16 +6690,22 @@
       <c r="S88" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="89" spans="1:19">
-      <c r="A89" s="2" t="s">
+      <c r="T88" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U88" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21">
+      <c r="A89" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>196</v>
+      <c r="C89" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>198</v>
@@ -6393,8 +6713,8 @@
       <c r="E89" s="3">
         <v>1</v>
       </c>
-      <c r="F89" s="2" t="s">
-        <v>196</v>
+      <c r="F89" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G89" s="3">
         <v>5</v>
@@ -6411,23 +6731,21 @@
       <c r="K89" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L89" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O89" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P89" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q89" s="5" t="s">
-        <v>196</v>
+      <c r="L89" s="5">
+        <v>2</v>
+      </c>
+      <c r="M89" s="5"/>
+      <c r="N89" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O89" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="P89" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q89" s="5">
+        <v>2</v>
       </c>
       <c r="R89" s="5" t="s">
         <v>196</v>
@@ -6435,16 +6753,22 @@
       <c r="S89" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="90" spans="1:19">
-      <c r="A90" s="2" t="s">
+      <c r="T89" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U89" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21">
+      <c r="A90" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>196</v>
+      <c r="C90" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>198</v>
@@ -6452,8 +6776,8 @@
       <c r="E90" s="3">
         <v>1</v>
       </c>
-      <c r="F90" s="2" t="s">
-        <v>196</v>
+      <c r="F90" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="G90" s="3">
         <v>7</v>
@@ -6470,28 +6794,32 @@
       <c r="K90" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L90" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N90" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O90" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="P90" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q90" s="5" t="s">
-        <v>196</v>
+      <c r="L90" s="5">
+        <v>2</v>
+      </c>
+      <c r="M90" s="5"/>
+      <c r="N90" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O90" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="P90" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q90" s="5">
+        <v>2</v>
       </c>
       <c r="R90" s="5" t="s">
         <v>196</v>
       </c>
       <c r="S90" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="T90" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U90" s="5" t="s">
         <v>196</v>
       </c>
     </row>

</xml_diff>